<commit_message>
add arquivos readme para CA e PM, formatando cronograma Excel, add links git
</commit_message>
<xml_diff>
--- a/PM/Cronograma/cronograma.xlsx
+++ b/PM/Cronograma/cronograma.xlsx
@@ -227,7 +227,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -256,30 +256,10 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
       <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -305,17 +285,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -339,42 +308,107 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -671,8 +705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -688,795 +722,795 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="16" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="9" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="3" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="25">
         <v>42704.333333333336</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="1">
         <v>42765.708333333336</v>
       </c>
-      <c r="I2" s="17"/>
+      <c r="I2" s="20"/>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="7" t="s">
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="26">
         <v>42704.333333333336</v>
       </c>
-      <c r="H3" s="8">
+      <c r="H3" s="18">
         <v>42713.708333333336</v>
       </c>
-      <c r="I3" s="18"/>
+      <c r="I3" s="21"/>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="5"/>
-      <c r="B4" s="7" t="s">
+      <c r="A4" s="2"/>
+      <c r="B4" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="7" t="s">
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="27">
         <v>42704.333333333336</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4" s="4">
         <v>42713.708333333336</v>
       </c>
-      <c r="I4" s="18"/>
+      <c r="I4" s="22"/>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="5"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7" t="s">
+      <c r="A5" s="15"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="26">
         <v>42704.333333333336</v>
       </c>
-      <c r="H5" s="8">
+      <c r="H5" s="18">
         <v>42713.708333333336</v>
       </c>
-      <c r="I5" s="18"/>
+      <c r="I5" s="21"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="5"/>
-      <c r="B6" s="7" t="s">
+      <c r="A6" s="2"/>
+      <c r="B6" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="7" t="s">
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="27">
         <v>42706.333333333336</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="4">
         <v>42713.708333333336</v>
       </c>
-      <c r="I6" s="18"/>
+      <c r="I6" s="22"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="5"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7" t="s">
+      <c r="A7" s="15"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="26">
         <v>42706.333333333336</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7" s="18">
         <v>42713.708333333336</v>
       </c>
-      <c r="I7" s="18"/>
+      <c r="I7" s="21"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="5"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7" t="s">
+      <c r="A8" s="15"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="26">
         <v>42706.333333333336</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8" s="18">
         <v>42713.708333333336</v>
       </c>
-      <c r="I8" s="18"/>
+      <c r="I8" s="21"/>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="7" t="s">
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="27">
         <v>42706.333333333336</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="4">
         <v>42765.708333333336</v>
       </c>
-      <c r="I9" s="18"/>
+      <c r="I9" s="22"/>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="5"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="6" t="s">
+      <c r="A10" s="15"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="7" t="s">
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="26">
         <v>42706.333333333336</v>
       </c>
-      <c r="H10" s="8">
+      <c r="H10" s="18">
         <v>42711.708333333336</v>
       </c>
-      <c r="I10" s="18"/>
+      <c r="I10" s="21"/>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="5"/>
-      <c r="B11" s="7" t="s">
+      <c r="A11" s="2"/>
+      <c r="B11" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="7" t="s">
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="27">
         <v>42706.333333333336</v>
       </c>
-      <c r="H11" s="8">
+      <c r="H11" s="4">
         <v>42765.708333333336</v>
       </c>
-      <c r="I11" s="18"/>
+      <c r="I11" s="22"/>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="5"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7" t="s">
+      <c r="A12" s="15"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="F12" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="26">
         <v>42706.333333333336</v>
       </c>
-      <c r="H12" s="8">
+      <c r="H12" s="18">
         <v>42711.708333333336</v>
       </c>
-      <c r="I12" s="18"/>
+      <c r="I12" s="21"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="5"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7" t="s">
+      <c r="A13" s="2"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G13" s="27">
         <v>42711.333333333336</v>
       </c>
-      <c r="H13" s="8">
+      <c r="H13" s="4">
         <v>42765.708333333336</v>
       </c>
-      <c r="I13" s="18"/>
+      <c r="I13" s="22"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="7" t="s">
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="G14" s="8">
+      <c r="G14" s="26">
         <v>42706.333333333336</v>
       </c>
-      <c r="H14" s="8">
+      <c r="H14" s="18">
         <v>42760.708333333336</v>
       </c>
-      <c r="I14" s="18"/>
+      <c r="I14" s="21"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="5"/>
-      <c r="B15" s="7" t="s">
+      <c r="A15" s="2"/>
+      <c r="B15" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="7" t="s">
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="8">
+      <c r="G15" s="27">
         <v>42706.333333333336</v>
       </c>
-      <c r="H15" s="8">
+      <c r="H15" s="4">
         <v>42716.708333333336</v>
       </c>
-      <c r="I15" s="18"/>
+      <c r="I15" s="22"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="5"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7" t="s">
+      <c r="A16" s="15"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F16" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G16" s="26">
         <v>42706.333333333336</v>
       </c>
-      <c r="H16" s="8">
+      <c r="H16" s="18">
         <v>42716.708333333336</v>
       </c>
-      <c r="I16" s="18"/>
+      <c r="I16" s="21"/>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="5"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7" t="s">
+      <c r="A17" s="2"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F17" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="G17" s="8">
+      <c r="G17" s="27">
         <v>42706.333333333336</v>
       </c>
-      <c r="H17" s="8">
+      <c r="H17" s="4">
         <v>42760.708333333336</v>
       </c>
-      <c r="I17" s="18"/>
+      <c r="I17" s="22"/>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="5"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7" t="s">
+      <c r="A18" s="15"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="F18" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="G18" s="8">
+      <c r="G18" s="26">
         <v>42706.333333333336</v>
       </c>
-      <c r="H18" s="8">
+      <c r="H18" s="18">
         <v>42760.708333333336</v>
       </c>
-      <c r="I18" s="18"/>
+      <c r="I18" s="21"/>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="5"/>
-      <c r="B19" s="7" t="s">
+      <c r="A19" s="2"/>
+      <c r="B19" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="7" t="s">
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="G19" s="8">
+      <c r="G19" s="27">
         <v>42717.333333333336</v>
       </c>
-      <c r="H19" s="8">
+      <c r="H19" s="4">
         <v>42723.708333333336</v>
       </c>
-      <c r="I19" s="18"/>
+      <c r="I19" s="22"/>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="5"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7" t="s">
+      <c r="A20" s="15"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="F20" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="G20" s="8">
+      <c r="G20" s="26">
         <v>42717.333333333336</v>
       </c>
-      <c r="H20" s="8">
+      <c r="H20" s="18">
         <v>42723.708333333336</v>
       </c>
-      <c r="I20" s="18"/>
+      <c r="I20" s="21"/>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="5"/>
-      <c r="B21" s="7" t="s">
+      <c r="A21" s="2"/>
+      <c r="B21" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="7" t="s">
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="G21" s="8">
+      <c r="G21" s="27">
         <v>42724.333333333336</v>
       </c>
-      <c r="H21" s="8">
+      <c r="H21" s="4">
         <v>42758.708333333336</v>
       </c>
-      <c r="I21" s="18"/>
+      <c r="I21" s="22"/>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="5"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="9" t="s">
+      <c r="A22" s="15"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="F22" s="7" t="s">
+      <c r="F22" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="G22" s="8">
+      <c r="G22" s="26">
         <v>42724.333333333336</v>
       </c>
-      <c r="H22" s="8">
+      <c r="H22" s="18">
         <v>42751.708333333336</v>
       </c>
-      <c r="I22" s="18"/>
+      <c r="I22" s="21"/>
     </row>
     <row r="23" spans="1:9">
-      <c r="A23" s="5"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7" t="s">
+      <c r="A23" s="2"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="F23" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="G23" s="8">
+      <c r="G23" s="27">
         <v>42752.333333333336</v>
       </c>
-      <c r="H23" s="8">
+      <c r="H23" s="4">
         <v>42758.708333333336</v>
       </c>
-      <c r="I23" s="18">
+      <c r="I23" s="22">
         <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:9">
-      <c r="A24" s="5"/>
-      <c r="B24" s="7" t="s">
+      <c r="A24" s="15"/>
+      <c r="B24" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="7" t="s">
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="G24" s="8">
+      <c r="G24" s="26">
         <v>42706.333333333336</v>
       </c>
-      <c r="H24" s="8">
+      <c r="H24" s="18">
         <v>42762.708333333336</v>
       </c>
-      <c r="I24" s="18"/>
+      <c r="I24" s="21"/>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="5"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7" t="s">
+      <c r="A25" s="2"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F25" s="7" t="s">
+      <c r="F25" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="G25" s="8">
+      <c r="G25" s="27">
         <v>42711.333333333336</v>
       </c>
-      <c r="H25" s="8">
+      <c r="H25" s="4">
         <v>42724.708333333336</v>
       </c>
-      <c r="I25" s="18"/>
+      <c r="I25" s="22"/>
     </row>
     <row r="26" spans="1:9">
-      <c r="A26" s="5"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7" t="s">
+      <c r="A26" s="15"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="F26" s="7" t="s">
+      <c r="F26" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G26" s="8">
+      <c r="G26" s="26">
         <v>42711.333333333336</v>
       </c>
-      <c r="H26" s="8">
+      <c r="H26" s="18">
         <v>42724.708333333336</v>
       </c>
-      <c r="I26" s="18"/>
+      <c r="I26" s="21"/>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="5"/>
-      <c r="B27" s="7" t="s">
+      <c r="A27" s="2"/>
+      <c r="B27" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="7" t="s">
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="G27" s="8">
+      <c r="G27" s="27">
         <v>42711.333333333336</v>
       </c>
-      <c r="H27" s="8">
+      <c r="H27" s="4">
         <v>42733.708333333336</v>
       </c>
-      <c r="I27" s="18"/>
+      <c r="I27" s="22"/>
     </row>
     <row r="28" spans="1:9">
-      <c r="A28" s="5"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7" t="s">
+      <c r="A28" s="15"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="F28" s="7" t="s">
+      <c r="F28" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="G28" s="8">
+      <c r="G28" s="26">
         <v>42711.333333333336</v>
       </c>
-      <c r="H28" s="8">
+      <c r="H28" s="18">
         <v>42719.708333333336</v>
       </c>
-      <c r="I28" s="18"/>
+      <c r="I28" s="21"/>
     </row>
     <row r="29" spans="1:9">
-      <c r="A29" s="5"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7" t="s">
+      <c r="A29" s="2"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F29" s="7" t="s">
+      <c r="F29" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="G29" s="8">
+      <c r="G29" s="27">
         <v>42720.333333333336</v>
       </c>
-      <c r="H29" s="8">
+      <c r="H29" s="4">
         <v>42733.708333333336</v>
       </c>
-      <c r="I29" s="18">
+      <c r="I29" s="22">
         <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:9">
-      <c r="A30" s="5"/>
-      <c r="B30" s="7" t="s">
+      <c r="A30" s="15"/>
+      <c r="B30" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C30" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="7" t="s">
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="G30" s="8">
+      <c r="G30" s="26">
         <v>42706.333333333336</v>
       </c>
-      <c r="H30" s="8">
+      <c r="H30" s="18">
         <v>42760.708333333336</v>
       </c>
-      <c r="I30" s="18"/>
+      <c r="I30" s="21"/>
     </row>
     <row r="31" spans="1:9">
-      <c r="A31" s="5"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7" t="s">
+      <c r="A31" s="2"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F31" s="7" t="s">
+      <c r="F31" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="G31" s="8">
+      <c r="G31" s="27">
         <v>42706.333333333336</v>
       </c>
-      <c r="H31" s="8">
+      <c r="H31" s="4">
         <v>42760.708333333336</v>
       </c>
-      <c r="I31" s="18"/>
+      <c r="I31" s="22"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="5"/>
-      <c r="B32" s="7" t="s">
+      <c r="A32" s="15"/>
+      <c r="B32" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C32" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="7" t="s">
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="G32" s="8">
+      <c r="G32" s="26">
         <v>42737.333333333336</v>
       </c>
-      <c r="H32" s="8">
+      <c r="H32" s="18">
         <v>42762.708333333336</v>
       </c>
-      <c r="I32" s="18"/>
+      <c r="I32" s="21"/>
     </row>
     <row r="33" spans="1:9">
-      <c r="A33" s="5"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="6" t="s">
+      <c r="A33" s="2"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="E33" s="6"/>
-      <c r="F33" s="7" t="s">
+      <c r="E33" s="11"/>
+      <c r="F33" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="G33" s="8">
+      <c r="G33" s="27">
         <v>42737.333333333336</v>
       </c>
-      <c r="H33" s="8">
+      <c r="H33" s="4">
         <v>42762.708333333336</v>
       </c>
-      <c r="I33" s="18"/>
+      <c r="I33" s="22"/>
     </row>
     <row r="34" spans="1:9">
-      <c r="A34" s="5"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7" t="s">
+      <c r="A34" s="15"/>
+      <c r="B34" s="17"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="F34" s="7" t="s">
+      <c r="F34" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="G34" s="8">
+      <c r="G34" s="26">
         <v>42737.333333333336</v>
       </c>
-      <c r="H34" s="8">
+      <c r="H34" s="18">
         <v>42755.708333333336</v>
       </c>
-      <c r="I34" s="18"/>
+      <c r="I34" s="21"/>
     </row>
     <row r="35" spans="1:9">
-      <c r="A35" s="5"/>
-      <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7" t="s">
+      <c r="A35" s="2"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F35" s="7" t="s">
+      <c r="F35" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="G35" s="8">
+      <c r="G35" s="27">
         <v>42758.333333333336</v>
       </c>
-      <c r="H35" s="8">
+      <c r="H35" s="4">
         <v>42762.708333333336</v>
       </c>
-      <c r="I35" s="18">
+      <c r="I35" s="22">
         <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:9">
-      <c r="A36" s="5"/>
-      <c r="B36" s="7" t="s">
+      <c r="A36" s="15"/>
+      <c r="B36" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C36" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="7" t="s">
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="G36" s="8">
+      <c r="G36" s="26">
         <v>42755.333333333336</v>
       </c>
-      <c r="H36" s="8">
+      <c r="H36" s="18">
         <v>42762.708333333336</v>
       </c>
-      <c r="I36" s="18"/>
+      <c r="I36" s="21"/>
     </row>
     <row r="37" spans="1:9">
-      <c r="A37" s="5"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7" t="s">
+      <c r="A37" s="2"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F37" s="7" t="s">
+      <c r="F37" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="G37" s="8">
+      <c r="G37" s="27">
         <v>42755.333333333336</v>
       </c>
-      <c r="H37" s="8">
+      <c r="H37" s="4">
         <v>42755.708333333336</v>
       </c>
-      <c r="I37" s="18"/>
+      <c r="I37" s="22"/>
     </row>
     <row r="38" spans="1:9">
-      <c r="A38" s="5"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7" t="s">
+      <c r="A38" s="15"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="17"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="F38" s="7" t="s">
+      <c r="F38" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="G38" s="8">
+      <c r="G38" s="26">
         <v>42762.333333333336</v>
       </c>
-      <c r="H38" s="8">
+      <c r="H38" s="18">
         <v>42762.708333333336</v>
       </c>
-      <c r="I38" s="18"/>
+      <c r="I38" s="21"/>
     </row>
     <row r="39" spans="1:9">
-      <c r="A39" s="11"/>
-      <c r="B39" s="12"/>
-      <c r="C39" s="13" t="s">
+      <c r="A39" s="6"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="D39" s="13"/>
-      <c r="E39" s="13"/>
-      <c r="F39" s="12" t="s">
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="G39" s="14">
+      <c r="G39" s="28">
         <v>42765.333333333336</v>
       </c>
-      <c r="H39" s="14">
+      <c r="H39" s="8">
         <v>42765.708333333336</v>
       </c>
-      <c r="I39" s="19"/>
+      <c r="I39" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="D33:E33"/>
     <mergeCell ref="C39:E39"/>
     <mergeCell ref="C15:E15"/>
     <mergeCell ref="C19:E19"/>
     <mergeCell ref="C21:E21"/>
     <mergeCell ref="C24:E24"/>
     <mergeCell ref="C27:E27"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="D33:E33"/>
     <mergeCell ref="C11:E11"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B14:E14"/>

</xml_diff>

<commit_message>
primeira revisão do cronograma
</commit_message>
<xml_diff>
--- a/PM/Cronograma/cronograma.xlsx
+++ b/PM/Cronograma/cronograma.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan1" sheetId="1" r:id="rId1"/>
+    <sheet name="cronograma" sheetId="1" r:id="rId1"/>
     <sheet name="Plan2" sheetId="2" r:id="rId2"/>
     <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="65">
   <si>
     <t>Projeto Robotino race</t>
   </si>
@@ -162,9 +162,6 @@
     <t>Integração dos módulos</t>
   </si>
   <si>
-    <t>Demostração do sistema</t>
-  </si>
-  <si>
     <t>Demonstração do protótipo preliminar</t>
   </si>
   <si>
@@ -193,13 +190,34 @@
   </si>
   <si>
     <t>Precedência</t>
+  </si>
+  <si>
+    <t>Legenda</t>
+  </si>
+  <si>
+    <t>Concluído</t>
+  </si>
+  <si>
+    <t>Replanejado</t>
+  </si>
+  <si>
+    <t>Crítico</t>
+  </si>
+  <si>
+    <t>Demonstração do sistema</t>
+  </si>
+  <si>
+    <t>11 dias</t>
+  </si>
+  <si>
+    <t>Atraso</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -212,8 +230,16 @@
       <color theme="1"/>
       <name val="ADMUI3Sm"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -223,6 +249,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -364,13 +420,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -378,35 +433,98 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -703,822 +821,958 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" customWidth="1"/>
-    <col min="3" max="3" width="6.140625" customWidth="1"/>
-    <col min="4" max="4" width="5.28515625" customWidth="1"/>
-    <col min="5" max="5" width="52.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" customWidth="1"/>
-    <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" customWidth="1"/>
+    <col min="3" max="3" width="7.140625" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" customWidth="1"/>
+    <col min="5" max="5" width="5.28515625" customWidth="1"/>
+    <col min="6" max="6" width="52.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" customWidth="1"/>
+    <col min="9" max="9" width="18" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" style="46" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.5703125" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:13">
+      <c r="B1" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1" s="48" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="H1" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="I1" s="9" t="s">
+      <c r="L1" s="47" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="13" t="s">
+      <c r="M1" s="47"/>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="45">
+        <v>1</v>
+      </c>
+      <c r="B2" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="20" t="s">
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="25">
+      <c r="H2" s="17">
         <v>42704.333333333336</v>
       </c>
-      <c r="H2" s="1">
+      <c r="I2" s="1">
         <v>42765.708333333336</v>
       </c>
-      <c r="I2" s="20"/>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="B3" s="16" t="s">
+      <c r="J2" s="49"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="45">
         <v>2</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="21" t="s">
+      <c r="B3" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="26">
+      <c r="H3" s="18">
         <v>42704.333333333336</v>
       </c>
-      <c r="H3" s="18">
+      <c r="I3" s="12">
         <v>42713.708333333336</v>
       </c>
-      <c r="I3" s="21"/>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" s="11" t="s">
+      <c r="J3" s="50"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="45">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="22" t="s">
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="27">
+      <c r="H4" s="19">
         <v>42704.333333333336</v>
       </c>
-      <c r="H4" s="4">
+      <c r="I4" s="4">
         <v>42713.708333333336</v>
       </c>
-      <c r="I4" s="22"/>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="15"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17" t="s">
+      <c r="J4" s="51"/>
+      <c r="L4" s="42"/>
+      <c r="M4" s="14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="45">
+        <v>4</v>
+      </c>
+      <c r="B5" s="33"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="21" t="s">
+      <c r="G5" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="26">
+      <c r="H5" s="36">
         <v>42704.333333333336</v>
       </c>
-      <c r="H5" s="18">
+      <c r="I5" s="37">
         <v>42713.708333333336</v>
       </c>
-      <c r="I5" s="21"/>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="2"/>
-      <c r="B6" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" s="11" t="s">
+      <c r="J5" s="52"/>
+      <c r="L5" s="39"/>
+      <c r="M5" s="14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="45">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="22" t="s">
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="27">
+      <c r="H6" s="19">
         <v>42706.333333333336</v>
       </c>
-      <c r="H6" s="4">
+      <c r="I6" s="4">
         <v>42713.708333333336</v>
       </c>
-      <c r="I6" s="22"/>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="15"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17" t="s">
+      <c r="J6" s="51"/>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="45">
+        <v>6</v>
+      </c>
+      <c r="B7" s="33"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="21" t="s">
+      <c r="G7" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="26">
+      <c r="H7" s="36">
         <v>42706.333333333336</v>
       </c>
-      <c r="H7" s="18">
+      <c r="I7" s="37">
         <v>42713.708333333336</v>
       </c>
-      <c r="I7" s="21"/>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="15"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17" t="s">
+      <c r="J7" s="52"/>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="45">
+        <v>7</v>
+      </c>
+      <c r="B8" s="33"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="21" t="s">
+      <c r="G8" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="26">
+      <c r="H8" s="36">
         <v>42706.333333333336</v>
       </c>
-      <c r="H8" s="18">
+      <c r="I8" s="37">
         <v>42713.708333333336</v>
       </c>
-      <c r="I8" s="21"/>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B9" s="11" t="s">
+      <c r="J8" s="52"/>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="45">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="22" t="s">
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="27">
+      <c r="H9" s="19">
         <v>42706.333333333336</v>
       </c>
-      <c r="H9" s="4">
+      <c r="I9" s="4">
         <v>42765.708333333336</v>
       </c>
-      <c r="I9" s="22"/>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="15"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="16" t="s">
+      <c r="J9" s="51"/>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="45">
+        <v>9</v>
+      </c>
+      <c r="B10" s="33"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="21" t="s">
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="26">
+      <c r="H10" s="36">
         <v>42706.333333333336</v>
       </c>
-      <c r="H10" s="18">
+      <c r="I10" s="37">
         <v>42711.708333333336</v>
       </c>
-      <c r="I10" s="21"/>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="2"/>
-      <c r="B11" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" s="11" t="s">
+      <c r="J10" s="52"/>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="45">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="22" t="s">
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="27">
+      <c r="H11" s="19">
         <v>42706.333333333336</v>
       </c>
-      <c r="H11" s="4">
+      <c r="I11" s="4">
         <v>42765.708333333336</v>
       </c>
-      <c r="I11" s="22"/>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="15"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17" t="s">
+      <c r="J11" s="51"/>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="45">
+        <v>11</v>
+      </c>
+      <c r="B12" s="33"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="21" t="s">
+      <c r="G12" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="26">
+      <c r="H12" s="36">
         <v>42706.333333333336</v>
       </c>
-      <c r="H12" s="18">
+      <c r="I12" s="37">
         <v>42711.708333333336</v>
       </c>
-      <c r="I12" s="21"/>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="2"/>
-      <c r="B13" s="3"/>
+      <c r="J12" s="52"/>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="45">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="3"/>
+      <c r="F13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="22" t="s">
+      <c r="G13" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="27">
+      <c r="H13" s="19">
         <v>42711.333333333336</v>
       </c>
-      <c r="H13" s="4">
+      <c r="I13" s="4">
         <v>42765.708333333336</v>
       </c>
-      <c r="I13" s="22"/>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="B14" s="16" t="s">
+      <c r="J13" s="51"/>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="45">
+        <v>13</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="21" t="s">
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="G14" s="26">
+      <c r="H14" s="18">
         <v>42706.333333333336</v>
       </c>
-      <c r="H14" s="18">
+      <c r="I14" s="12">
         <v>42760.708333333336</v>
       </c>
-      <c r="I14" s="21"/>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="2"/>
-      <c r="B15" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C15" s="11" t="s">
+      <c r="J14" s="50"/>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="45">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="22" t="s">
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="27">
+      <c r="H15" s="19">
         <v>42706.333333333336</v>
       </c>
-      <c r="H15" s="4">
+      <c r="I15" s="4">
+        <v>42394.708333333336</v>
+      </c>
+      <c r="J15" s="51"/>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="45">
+        <v>15</v>
+      </c>
+      <c r="B16" s="28"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="H16" s="31">
+        <v>42706.333333333336</v>
+      </c>
+      <c r="I16" s="32">
         <v>42716.708333333336</v>
       </c>
-      <c r="I15" s="22"/>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="15"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="F16" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="G16" s="26">
-        <v>42706.333333333336</v>
-      </c>
-      <c r="H16" s="18">
-        <v>42716.708333333336</v>
-      </c>
-      <c r="I16" s="21"/>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="2"/>
-      <c r="B17" s="3"/>
+      <c r="J16" s="53"/>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="45">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="3"/>
+      <c r="F17" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F17" s="22" t="s">
+      <c r="G17" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="G17" s="27">
+      <c r="H17" s="19">
         <v>42706.333333333336</v>
       </c>
-      <c r="H17" s="4">
+      <c r="I17" s="4">
         <v>42760.708333333336</v>
       </c>
-      <c r="I17" s="22"/>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="15"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17" t="s">
+      <c r="J17" s="51"/>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="45">
+        <v>17</v>
+      </c>
+      <c r="B18" s="10"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F18" s="21" t="s">
+      <c r="G18" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="G18" s="26">
+      <c r="H18" s="18">
         <v>42706.333333333336</v>
       </c>
-      <c r="H18" s="18">
+      <c r="I18" s="12">
         <v>42760.708333333336</v>
       </c>
-      <c r="I18" s="21"/>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="2"/>
-      <c r="B19" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C19" s="11" t="s">
+      <c r="J18" s="50"/>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="45">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="22" t="s">
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="G19" s="27">
+      <c r="H19" s="19">
         <v>42717.333333333336</v>
       </c>
-      <c r="H19" s="4">
-        <v>42723.708333333336</v>
-      </c>
-      <c r="I19" s="22"/>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="15"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17" t="s">
+      <c r="I19" s="4">
+        <v>42374.708333333336</v>
+      </c>
+      <c r="J19" s="51"/>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="45">
+        <v>19</v>
+      </c>
+      <c r="B20" s="40"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="F20" s="21" t="s">
+      <c r="G20" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="G20" s="26">
-        <v>42717.333333333336</v>
-      </c>
-      <c r="H20" s="18">
-        <v>42723.708333333336</v>
-      </c>
-      <c r="I20" s="21"/>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="2"/>
-      <c r="B21" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C21" s="11" t="s">
+      <c r="H20" s="43">
+        <v>42733.333333333336</v>
+      </c>
+      <c r="I20" s="44">
+        <v>42374.708333333336</v>
+      </c>
+      <c r="J20" s="54"/>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="45">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="22" t="s">
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="G21" s="27">
+      <c r="H21" s="19">
         <v>42724.333333333336</v>
       </c>
-      <c r="H21" s="4">
+      <c r="I21" s="4">
         <v>42758.708333333336</v>
       </c>
-      <c r="I21" s="22"/>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="A22" s="15"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="19" t="s">
+      <c r="J21" s="51"/>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="45">
+        <v>21</v>
+      </c>
+      <c r="B22" s="40"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="F22" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="G22" s="26">
-        <v>42724.333333333336</v>
-      </c>
-      <c r="H22" s="18">
+      <c r="G22" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="H22" s="43">
+        <v>42737.333333333336</v>
+      </c>
+      <c r="I22" s="44">
         <v>42751.708333333336</v>
       </c>
-      <c r="I22" s="21"/>
-    </row>
-    <row r="23" spans="1:9">
-      <c r="A23" s="2"/>
-      <c r="B23" s="3"/>
+      <c r="J22" s="54"/>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="45">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="3" t="s">
+      <c r="E23" s="3"/>
+      <c r="F23" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F23" s="22" t="s">
+      <c r="G23" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="G23" s="27">
+      <c r="H23" s="19">
         <v>42752.333333333336</v>
       </c>
-      <c r="H23" s="4">
+      <c r="I23" s="4">
         <v>42758.708333333336</v>
       </c>
-      <c r="I23" s="22">
+      <c r="J23" s="51">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
-      <c r="A24" s="15"/>
-      <c r="B24" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="C24" s="16" t="s">
+    <row r="24" spans="1:10">
+      <c r="A24" s="45">
+        <v>23</v>
+      </c>
+      <c r="B24" s="10"/>
+      <c r="C24" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="21" t="s">
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="G24" s="26">
+      <c r="H24" s="18">
         <v>42706.333333333336</v>
       </c>
-      <c r="H24" s="18">
+      <c r="I24" s="12">
         <v>42762.708333333336</v>
       </c>
-      <c r="I24" s="21"/>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="A25" s="2"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3" t="s">
+      <c r="J24" s="50"/>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="45">
+        <v>24</v>
+      </c>
+      <c r="B25" s="57"/>
+      <c r="C25" s="58"/>
+      <c r="D25" s="59"/>
+      <c r="E25" s="58"/>
+      <c r="F25" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="F25" s="22" t="s">
+      <c r="G25" s="60" t="s">
         <v>35</v>
       </c>
-      <c r="G25" s="27">
+      <c r="H25" s="61">
         <v>42711.333333333336</v>
       </c>
-      <c r="H25" s="4">
-        <v>42724.708333333336</v>
-      </c>
-      <c r="I25" s="22"/>
-    </row>
-    <row r="26" spans="1:9">
-      <c r="A26" s="15"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17" t="s">
+      <c r="I25" s="62">
+        <v>42731.708333333336</v>
+      </c>
+      <c r="J25" s="63"/>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="45">
+        <v>25</v>
+      </c>
+      <c r="B26" s="40"/>
+      <c r="C26" s="41"/>
+      <c r="D26" s="41"/>
+      <c r="E26" s="41"/>
+      <c r="F26" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="F26" s="21" t="s">
+      <c r="G26" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="G26" s="26">
+      <c r="H26" s="43">
         <v>42711.333333333336</v>
       </c>
-      <c r="H26" s="18">
-        <v>42724.708333333336</v>
-      </c>
-      <c r="I26" s="21"/>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="A27" s="2"/>
-      <c r="B27" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C27" s="11" t="s">
+      <c r="I26" s="44">
+        <v>42731.708333333336</v>
+      </c>
+      <c r="J26" s="54"/>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="45">
+        <v>26</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="22" t="s">
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="G27" s="27">
+      <c r="H27" s="19">
         <v>42711.333333333336</v>
       </c>
-      <c r="H27" s="4">
+      <c r="I27" s="4">
+        <v>42371.708333333336</v>
+      </c>
+      <c r="J27" s="51"/>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="45">
+        <v>27</v>
+      </c>
+      <c r="B28" s="40"/>
+      <c r="C28" s="41"/>
+      <c r="D28" s="41"/>
+      <c r="E28" s="41"/>
+      <c r="F28" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="G28" s="42" t="s">
+        <v>20</v>
+      </c>
+      <c r="H28" s="43">
+        <v>42711.333333333336</v>
+      </c>
+      <c r="I28" s="44">
         <v>42733.708333333336</v>
       </c>
-      <c r="I27" s="22"/>
-    </row>
-    <row r="28" spans="1:9">
-      <c r="A28" s="15"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="F28" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="G28" s="26">
-        <v>42711.333333333336</v>
-      </c>
-      <c r="H28" s="18">
-        <v>42719.708333333336</v>
-      </c>
-      <c r="I28" s="21"/>
-    </row>
-    <row r="29" spans="1:9">
-      <c r="A29" s="2"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3" t="s">
+      <c r="J28" s="54"/>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="45">
+        <v>28</v>
+      </c>
+      <c r="B29" s="57"/>
+      <c r="C29" s="58"/>
+      <c r="D29" s="58"/>
+      <c r="E29" s="58"/>
+      <c r="F29" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="F29" s="22" t="s">
+      <c r="G29" s="60" t="s">
         <v>35</v>
       </c>
-      <c r="G29" s="27">
+      <c r="H29" s="61">
         <v>42720.333333333336</v>
       </c>
-      <c r="H29" s="4">
-        <v>42733.708333333336</v>
-      </c>
-      <c r="I29" s="22">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
-      <c r="A30" s="15"/>
-      <c r="B30" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="C30" s="16" t="s">
+      <c r="I29" s="62">
+        <v>42371.708333333336</v>
+      </c>
+      <c r="J29" s="63"/>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="45">
+        <v>29</v>
+      </c>
+      <c r="B30" s="10"/>
+      <c r="C30" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D30" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="21" t="s">
+      <c r="E30" s="23"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="G30" s="26">
+      <c r="H30" s="18">
         <v>42706.333333333336</v>
       </c>
-      <c r="H30" s="18">
+      <c r="I30" s="12">
         <v>42760.708333333336</v>
       </c>
-      <c r="I30" s="21"/>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="A31" s="2"/>
-      <c r="B31" s="3"/>
+      <c r="J30" s="50"/>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" s="45">
+        <v>30</v>
+      </c>
+      <c r="B31" s="2"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
-      <c r="E31" s="3" t="s">
+      <c r="E31" s="3"/>
+      <c r="F31" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F31" s="22" t="s">
+      <c r="G31" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="G31" s="27">
+      <c r="H31" s="19">
         <v>42706.333333333336</v>
       </c>
-      <c r="H31" s="4">
+      <c r="I31" s="4">
         <v>42760.708333333336</v>
       </c>
-      <c r="I31" s="22"/>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="A32" s="15"/>
-      <c r="B32" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="C32" s="16" t="s">
+      <c r="J31" s="51"/>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" s="45">
+        <v>31</v>
+      </c>
+      <c r="B32" s="10"/>
+      <c r="C32" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D32" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="D32" s="16"/>
-      <c r="E32" s="16"/>
-      <c r="F32" s="21" t="s">
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="G32" s="26">
+      <c r="H32" s="18">
         <v>42737.333333333336</v>
       </c>
-      <c r="H32" s="18">
+      <c r="I32" s="12">
         <v>42762.708333333336</v>
       </c>
-      <c r="I32" s="21"/>
-    </row>
-    <row r="33" spans="1:9">
-      <c r="A33" s="2"/>
-      <c r="B33" s="3"/>
+      <c r="J32" s="50"/>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="45">
+        <v>32</v>
+      </c>
+      <c r="B33" s="2"/>
       <c r="C33" s="3"/>
-      <c r="D33" s="11" t="s">
+      <c r="D33" s="3"/>
+      <c r="E33" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="E33" s="11"/>
-      <c r="F33" s="22" t="s">
+      <c r="F33" s="22"/>
+      <c r="G33" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="G33" s="27">
+      <c r="H33" s="19">
         <v>42737.333333333336</v>
       </c>
-      <c r="H33" s="4">
+      <c r="I33" s="4">
         <v>42762.708333333336</v>
       </c>
-      <c r="I33" s="22"/>
-    </row>
-    <row r="34" spans="1:9">
-      <c r="A34" s="15"/>
-      <c r="B34" s="17"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17" t="s">
+      <c r="J33" s="51"/>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" s="45">
+        <v>33</v>
+      </c>
+      <c r="B34" s="10"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="F34" s="21" t="s">
+      <c r="G34" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G34" s="26">
+      <c r="H34" s="18">
         <v>42737.333333333336</v>
       </c>
-      <c r="H34" s="18">
+      <c r="I34" s="12">
         <v>42755.708333333336</v>
       </c>
-      <c r="I34" s="21"/>
-    </row>
-    <row r="35" spans="1:9">
-      <c r="A35" s="2"/>
-      <c r="B35" s="3"/>
+      <c r="J34" s="50"/>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" s="45">
+        <v>34</v>
+      </c>
+      <c r="B35" s="2"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
-      <c r="E35" s="3" t="s">
+      <c r="E35" s="3"/>
+      <c r="F35" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F35" s="22" t="s">
+      <c r="G35" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="G35" s="27">
+      <c r="H35" s="19">
         <v>42758.333333333336</v>
       </c>
-      <c r="H35" s="4">
+      <c r="I35" s="4">
         <v>42762.708333333336</v>
       </c>
-      <c r="I35" s="22">
+      <c r="J35" s="51">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
-      <c r="A36" s="15"/>
-      <c r="B36" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="C36" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="D36" s="16"/>
-      <c r="E36" s="16"/>
-      <c r="F36" s="21" t="s">
+    <row r="36" spans="1:10">
+      <c r="A36" s="45">
+        <v>35</v>
+      </c>
+      <c r="B36" s="10"/>
+      <c r="C36" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D36" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
+      <c r="G36" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="G36" s="26">
+      <c r="H36" s="18">
         <v>42755.333333333336</v>
       </c>
-      <c r="H36" s="18">
+      <c r="I36" s="12">
         <v>42762.708333333336</v>
       </c>
-      <c r="I36" s="21"/>
-    </row>
-    <row r="37" spans="1:9">
-      <c r="A37" s="2"/>
-      <c r="B37" s="3"/>
+      <c r="J36" s="50"/>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" s="45">
+        <v>36</v>
+      </c>
+      <c r="B37" s="2"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
-      <c r="E37" s="3" t="s">
+      <c r="E37" s="3"/>
+      <c r="F37" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G37" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="F37" s="22" t="s">
+      <c r="H37" s="19">
+        <v>42755.333333333336</v>
+      </c>
+      <c r="I37" s="4">
+        <v>42755.708333333336</v>
+      </c>
+      <c r="J37" s="51"/>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" s="45">
+        <v>37</v>
+      </c>
+      <c r="B38" s="10"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="G37" s="27">
-        <v>42755.333333333336</v>
-      </c>
-      <c r="H37" s="4">
-        <v>42755.708333333336</v>
-      </c>
-      <c r="I37" s="22"/>
-    </row>
-    <row r="38" spans="1:9">
-      <c r="A38" s="15"/>
-      <c r="B38" s="17"/>
-      <c r="C38" s="17"/>
-      <c r="D38" s="17"/>
-      <c r="E38" s="17" t="s">
+      <c r="G38" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="H38" s="18">
+        <v>42762.333333333336</v>
+      </c>
+      <c r="I38" s="12">
+        <v>42762.708333333336</v>
+      </c>
+      <c r="J38" s="50"/>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="45">
+        <v>38</v>
+      </c>
+      <c r="B39" s="5"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="F38" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="G38" s="26">
-        <v>42762.333333333336</v>
-      </c>
-      <c r="H38" s="18">
-        <v>42762.708333333336</v>
-      </c>
-      <c r="I38" s="21"/>
-    </row>
-    <row r="39" spans="1:9">
-      <c r="A39" s="6"/>
-      <c r="B39" s="7"/>
-      <c r="C39" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="D39" s="12"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="G39" s="28">
+      <c r="E39" s="21"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="H39" s="20">
         <v>42765.333333333336</v>
       </c>
-      <c r="H39" s="8">
+      <c r="I39" s="7">
         <v>42765.708333333336</v>
       </c>
-      <c r="I39" s="23"/>
+      <c r="J39" s="55"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C6:E6"/>
+  <mergeCells count="20">
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D27:F27"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
revisão cronograma, sincronizar testes e codificação, dos modulos e integração do sistema
</commit_message>
<xml_diff>
--- a/PM/Cronograma/cronograma.xlsx
+++ b/PM/Cronograma/cronograma.xlsx
@@ -444,27 +444,6 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
@@ -475,9 +454,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
@@ -488,9 +464,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -526,6 +499,33 @@
     <xf numFmtId="22" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -823,8 +823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -837,47 +837,47 @@
     <col min="6" max="6" width="52.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.28515625" customWidth="1"/>
     <col min="9" max="9" width="18" customWidth="1"/>
-    <col min="10" max="10" width="11.85546875" style="46" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" style="38" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="4.5703125" customWidth="1"/>
     <col min="13" max="13" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="56" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="25"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="57"/>
       <c r="G1" s="8" t="s">
         <v>53</v>
       </c>
       <c r="H1" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="I1" s="48" t="s">
+      <c r="I1" s="39" t="s">
         <v>55</v>
       </c>
       <c r="J1" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="L1" s="47" t="s">
+      <c r="L1" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="M1" s="47"/>
+      <c r="M1" s="55"/>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="45">
+      <c r="A2" s="37">
         <v>1</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
       <c r="G2" s="13" t="s">
         <v>1</v>
       </c>
@@ -887,25 +887,25 @@
       <c r="I2" s="1">
         <v>42765.708333333336</v>
       </c>
-      <c r="J2" s="49"/>
-      <c r="L2" s="35"/>
+      <c r="J2" s="40"/>
+      <c r="L2" s="28"/>
       <c r="M2" s="14" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="45">
+      <c r="A3" s="37">
         <v>2</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
       <c r="G3" s="14" t="s">
         <v>3</v>
       </c>
@@ -915,25 +915,25 @@
       <c r="I3" s="12">
         <v>42713.708333333336</v>
       </c>
-      <c r="J3" s="50"/>
-      <c r="L3" s="30"/>
+      <c r="J3" s="41"/>
+      <c r="L3" s="23"/>
       <c r="M3" s="14" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="45">
+      <c r="A4" s="37">
         <v>3</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="59"/>
       <c r="G4" s="15" t="s">
         <v>3</v>
       </c>
@@ -943,51 +943,51 @@
       <c r="I4" s="4">
         <v>42713.708333333336</v>
       </c>
-      <c r="J4" s="51"/>
-      <c r="L4" s="42"/>
+      <c r="J4" s="42"/>
+      <c r="L4" s="34"/>
       <c r="M4" s="14" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="45">
+      <c r="A5" s="37">
         <v>4</v>
       </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34" t="s">
+      <c r="B5" s="26"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="35" t="s">
+      <c r="G5" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="36">
+      <c r="H5" s="29">
         <v>42704.333333333336</v>
       </c>
-      <c r="I5" s="37">
+      <c r="I5" s="30">
         <v>42713.708333333336</v>
       </c>
-      <c r="J5" s="52"/>
-      <c r="L5" s="39"/>
+      <c r="J5" s="43"/>
+      <c r="L5" s="31"/>
       <c r="M5" s="14" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="45">
+      <c r="A6" s="37">
         <v>5</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
+      <c r="E6" s="59"/>
+      <c r="F6" s="59"/>
       <c r="G6" s="15" t="s">
         <v>7</v>
       </c>
@@ -997,65 +997,65 @@
       <c r="I6" s="4">
         <v>42713.708333333336</v>
       </c>
-      <c r="J6" s="51"/>
+      <c r="J6" s="42"/>
     </row>
     <row r="7" spans="1:13">
-      <c r="A7" s="45">
+      <c r="A7" s="37">
         <v>6</v>
       </c>
-      <c r="B7" s="33"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34" t="s">
+      <c r="B7" s="26"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="35" t="s">
+      <c r="G7" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="36">
+      <c r="H7" s="29">
         <v>42706.333333333336</v>
       </c>
-      <c r="I7" s="37">
+      <c r="I7" s="30">
         <v>42713.708333333336</v>
       </c>
-      <c r="J7" s="52"/>
+      <c r="J7" s="43"/>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="45">
+      <c r="A8" s="37">
         <v>7</v>
       </c>
-      <c r="B8" s="33"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34" t="s">
+      <c r="B8" s="26"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="35" t="s">
+      <c r="G8" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="H8" s="36">
+      <c r="H8" s="29">
         <v>42706.333333333336</v>
       </c>
-      <c r="I8" s="37">
+      <c r="I8" s="30">
         <v>42713.708333333336</v>
       </c>
-      <c r="J8" s="52"/>
+      <c r="J8" s="43"/>
     </row>
     <row r="9" spans="1:13">
-      <c r="A9" s="45">
+      <c r="A9" s="37">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
+      <c r="D9" s="59"/>
+      <c r="E9" s="59"/>
+      <c r="F9" s="59"/>
       <c r="G9" s="15" t="s">
         <v>11</v>
       </c>
@@ -1065,43 +1065,43 @@
       <c r="I9" s="4">
         <v>42765.708333333336</v>
       </c>
-      <c r="J9" s="51"/>
+      <c r="J9" s="42"/>
     </row>
     <row r="10" spans="1:13">
-      <c r="A10" s="45">
+      <c r="A10" s="37">
         <v>9</v>
       </c>
-      <c r="B10" s="33"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="38" t="s">
+      <c r="B10" s="26"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="35" t="s">
+      <c r="E10" s="60"/>
+      <c r="F10" s="60"/>
+      <c r="G10" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="H10" s="36">
+      <c r="H10" s="29">
         <v>42706.333333333336</v>
       </c>
-      <c r="I10" s="37">
+      <c r="I10" s="30">
         <v>42711.708333333336</v>
       </c>
-      <c r="J10" s="52"/>
+      <c r="J10" s="43"/>
     </row>
     <row r="11" spans="1:13">
-      <c r="A11" s="45">
+      <c r="A11" s="37">
         <v>10</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="22" t="s">
+      <c r="D11" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="59"/>
       <c r="G11" s="15" t="s">
         <v>11</v>
       </c>
@@ -1111,32 +1111,32 @@
       <c r="I11" s="4">
         <v>42765.708333333336</v>
       </c>
-      <c r="J11" s="51"/>
+      <c r="J11" s="42"/>
     </row>
     <row r="12" spans="1:13">
-      <c r="A12" s="45">
+      <c r="A12" s="37">
         <v>11</v>
       </c>
-      <c r="B12" s="33"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34" t="s">
+      <c r="B12" s="26"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="35" t="s">
+      <c r="G12" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="H12" s="36">
+      <c r="H12" s="29">
         <v>42706.333333333336</v>
       </c>
-      <c r="I12" s="37">
+      <c r="I12" s="30">
         <v>42711.708333333336</v>
       </c>
-      <c r="J12" s="52"/>
+      <c r="J12" s="43"/>
     </row>
     <row r="13" spans="1:13">
-      <c r="A13" s="45">
+      <c r="A13" s="37">
         <v>12</v>
       </c>
       <c r="B13" s="2"/>
@@ -1155,21 +1155,21 @@
       <c r="I13" s="4">
         <v>42765.708333333336</v>
       </c>
-      <c r="J13" s="51"/>
+      <c r="J13" s="42"/>
     </row>
     <row r="14" spans="1:13">
-      <c r="A14" s="45">
+      <c r="A14" s="37">
         <v>13</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C14" s="23" t="s">
+      <c r="C14" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
+      <c r="D14" s="58"/>
+      <c r="E14" s="58"/>
+      <c r="F14" s="58"/>
       <c r="G14" s="14" t="s">
         <v>17</v>
       </c>
@@ -1179,21 +1179,21 @@
       <c r="I14" s="12">
         <v>42760.708333333336</v>
       </c>
-      <c r="J14" s="50"/>
+      <c r="J14" s="41"/>
     </row>
     <row r="15" spans="1:13">
-      <c r="A15" s="45">
+      <c r="A15" s="37">
         <v>14</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D15" s="22" t="s">
+      <c r="D15" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
+      <c r="E15" s="59"/>
+      <c r="F15" s="59"/>
       <c r="G15" s="15" t="s">
         <v>20</v>
       </c>
@@ -1203,32 +1203,32 @@
       <c r="I15" s="4">
         <v>42394.708333333336</v>
       </c>
-      <c r="J15" s="51"/>
+      <c r="J15" s="42"/>
     </row>
     <row r="16" spans="1:13">
-      <c r="A16" s="45">
+      <c r="A16" s="37">
         <v>15</v>
       </c>
-      <c r="B16" s="28"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29" t="s">
+      <c r="B16" s="21"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="G16" s="30" t="s">
+      <c r="G16" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="H16" s="31">
+      <c r="H16" s="24">
         <v>42706.333333333336</v>
       </c>
-      <c r="I16" s="32">
+      <c r="I16" s="25">
         <v>42716.708333333336</v>
       </c>
-      <c r="J16" s="53"/>
+      <c r="J16" s="44"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="45">
+      <c r="A17" s="37">
         <v>16</v>
       </c>
       <c r="B17" s="2"/>
@@ -1247,10 +1247,10 @@
       <c r="I17" s="4">
         <v>42760.708333333336</v>
       </c>
-      <c r="J17" s="51"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="45">
+      <c r="A18" s="37">
         <v>17</v>
       </c>
       <c r="B18" s="10"/>
@@ -1269,21 +1269,21 @@
       <c r="I18" s="12">
         <v>42760.708333333336</v>
       </c>
-      <c r="J18" s="50"/>
+      <c r="J18" s="41"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="45">
+      <c r="A19" s="37">
         <v>18</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D19" s="22" t="s">
+      <c r="D19" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
+      <c r="E19" s="59"/>
+      <c r="F19" s="59"/>
       <c r="G19" s="15" t="s">
         <v>25</v>
       </c>
@@ -1293,43 +1293,43 @@
       <c r="I19" s="4">
         <v>42374.708333333336</v>
       </c>
-      <c r="J19" s="51"/>
+      <c r="J19" s="42"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="45">
+      <c r="A20" s="37">
         <v>19</v>
       </c>
-      <c r="B20" s="40"/>
-      <c r="C20" s="41"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="41"/>
-      <c r="F20" s="41" t="s">
+      <c r="B20" s="32"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="G20" s="42" t="s">
+      <c r="G20" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="H20" s="43">
+      <c r="H20" s="35">
         <v>42733.333333333336</v>
       </c>
-      <c r="I20" s="44">
+      <c r="I20" s="36">
         <v>42374.708333333336</v>
       </c>
-      <c r="J20" s="54"/>
+      <c r="J20" s="45"/>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="45">
+      <c r="A21" s="37">
         <v>20</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="22" t="s">
+      <c r="D21" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="E21" s="22"/>
-      <c r="F21" s="22"/>
+      <c r="E21" s="59"/>
+      <c r="F21" s="59"/>
       <c r="G21" s="15" t="s">
         <v>28</v>
       </c>
@@ -1339,67 +1339,67 @@
       <c r="I21" s="4">
         <v>42758.708333333336</v>
       </c>
-      <c r="J21" s="51"/>
+      <c r="J21" s="42"/>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="45">
+      <c r="A22" s="37">
         <v>21</v>
       </c>
-      <c r="B22" s="40"/>
-      <c r="C22" s="41"/>
-      <c r="D22" s="41"/>
-      <c r="E22" s="41"/>
-      <c r="F22" s="56" t="s">
+      <c r="B22" s="32"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="33"/>
+      <c r="F22" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="G22" s="42" t="s">
+      <c r="G22" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="H22" s="43">
+      <c r="H22" s="35">
         <v>42737.333333333336</v>
       </c>
-      <c r="I22" s="44">
-        <v>42751.708333333336</v>
-      </c>
-      <c r="J22" s="54"/>
+      <c r="I22" s="36">
+        <v>42755.708333333336</v>
+      </c>
+      <c r="J22" s="45"/>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="45">
+      <c r="A23" s="37">
         <v>22</v>
       </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3" t="s">
+      <c r="B23" s="48"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="G23" s="15" t="s">
+      <c r="G23" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="H23" s="19">
-        <v>42752.333333333336</v>
-      </c>
-      <c r="I23" s="4">
-        <v>42758.708333333336</v>
-      </c>
-      <c r="J23" s="51">
+      <c r="H23" s="52">
+        <v>42758.333333333336</v>
+      </c>
+      <c r="I23" s="53">
+        <v>42762.708333333336</v>
+      </c>
+      <c r="J23" s="54">
         <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" s="45">
+      <c r="A24" s="37">
         <v>23</v>
       </c>
       <c r="B24" s="10"/>
       <c r="C24" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="D24" s="23" t="s">
+      <c r="D24" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="E24" s="23"/>
-      <c r="F24" s="23"/>
+      <c r="E24" s="58"/>
+      <c r="F24" s="58"/>
       <c r="G24" s="14" t="s">
         <v>33</v>
       </c>
@@ -1409,65 +1409,65 @@
       <c r="I24" s="12">
         <v>42762.708333333336</v>
       </c>
-      <c r="J24" s="50"/>
+      <c r="J24" s="41"/>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="45">
+      <c r="A25" s="37">
         <v>24</v>
       </c>
-      <c r="B25" s="57"/>
-      <c r="C25" s="58"/>
-      <c r="D25" s="59"/>
-      <c r="E25" s="58"/>
-      <c r="F25" s="58" t="s">
+      <c r="B25" s="48"/>
+      <c r="C25" s="49"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="G25" s="60" t="s">
+      <c r="G25" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="H25" s="61">
+      <c r="H25" s="52">
         <v>42711.333333333336</v>
       </c>
-      <c r="I25" s="62">
+      <c r="I25" s="53">
         <v>42731.708333333336</v>
       </c>
-      <c r="J25" s="63"/>
+      <c r="J25" s="54"/>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="45">
+      <c r="A26" s="37">
         <v>25</v>
       </c>
-      <c r="B26" s="40"/>
-      <c r="C26" s="41"/>
-      <c r="D26" s="41"/>
-      <c r="E26" s="41"/>
-      <c r="F26" s="41" t="s">
+      <c r="B26" s="32"/>
+      <c r="C26" s="33"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="G26" s="42" t="s">
+      <c r="G26" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="H26" s="43">
+      <c r="H26" s="35">
         <v>42711.333333333336</v>
       </c>
-      <c r="I26" s="44">
+      <c r="I26" s="36">
         <v>42731.708333333336</v>
       </c>
-      <c r="J26" s="54"/>
+      <c r="J26" s="45"/>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="45">
+      <c r="A27" s="37">
         <v>26</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D27" s="22" t="s">
+      <c r="D27" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
+      <c r="E27" s="59"/>
+      <c r="F27" s="59"/>
       <c r="G27" s="15" t="s">
         <v>38</v>
       </c>
@@ -1477,65 +1477,65 @@
       <c r="I27" s="4">
         <v>42371.708333333336</v>
       </c>
-      <c r="J27" s="51"/>
+      <c r="J27" s="42"/>
     </row>
     <row r="28" spans="1:10">
-      <c r="A28" s="45">
+      <c r="A28" s="37">
         <v>27</v>
       </c>
-      <c r="B28" s="40"/>
-      <c r="C28" s="41"/>
-      <c r="D28" s="41"/>
-      <c r="E28" s="41"/>
-      <c r="F28" s="41" t="s">
+      <c r="B28" s="32"/>
+      <c r="C28" s="33"/>
+      <c r="D28" s="33"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="G28" s="42" t="s">
+      <c r="G28" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="H28" s="43">
+      <c r="H28" s="35">
         <v>42711.333333333336</v>
       </c>
-      <c r="I28" s="44">
+      <c r="I28" s="36">
         <v>42733.708333333336</v>
       </c>
-      <c r="J28" s="54"/>
+      <c r="J28" s="45"/>
     </row>
     <row r="29" spans="1:10">
-      <c r="A29" s="45">
+      <c r="A29" s="37">
         <v>28</v>
       </c>
-      <c r="B29" s="57"/>
-      <c r="C29" s="58"/>
-      <c r="D29" s="58"/>
-      <c r="E29" s="58"/>
-      <c r="F29" s="58" t="s">
+      <c r="B29" s="48"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="49"/>
+      <c r="E29" s="49"/>
+      <c r="F29" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="G29" s="60" t="s">
+      <c r="G29" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="H29" s="61">
+      <c r="H29" s="52">
         <v>42720.333333333336</v>
       </c>
-      <c r="I29" s="62">
+      <c r="I29" s="53">
         <v>42371.708333333336</v>
       </c>
-      <c r="J29" s="63"/>
+      <c r="J29" s="54"/>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="45">
+      <c r="A30" s="37">
         <v>29</v>
       </c>
       <c r="B30" s="10"/>
       <c r="C30" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="D30" s="23" t="s">
+      <c r="D30" s="58" t="s">
         <v>41</v>
       </c>
-      <c r="E30" s="23"/>
-      <c r="F30" s="23"/>
+      <c r="E30" s="58"/>
+      <c r="F30" s="58"/>
       <c r="G30" s="14" t="s">
         <v>17</v>
       </c>
@@ -1545,10 +1545,10 @@
       <c r="I30" s="12">
         <v>42760.708333333336</v>
       </c>
-      <c r="J30" s="50"/>
+      <c r="J30" s="41"/>
     </row>
     <row r="31" spans="1:10">
-      <c r="A31" s="45">
+      <c r="A31" s="37">
         <v>30</v>
       </c>
       <c r="B31" s="2"/>
@@ -1567,21 +1567,21 @@
       <c r="I31" s="4">
         <v>42760.708333333336</v>
       </c>
-      <c r="J31" s="51"/>
+      <c r="J31" s="42"/>
     </row>
     <row r="32" spans="1:10">
-      <c r="A32" s="45">
+      <c r="A32" s="37">
         <v>31</v>
       </c>
       <c r="B32" s="10"/>
       <c r="C32" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="D32" s="23" t="s">
+      <c r="D32" s="58" t="s">
         <v>43</v>
       </c>
-      <c r="E32" s="23"/>
-      <c r="F32" s="23"/>
+      <c r="E32" s="58"/>
+      <c r="F32" s="58"/>
       <c r="G32" s="14" t="s">
         <v>30</v>
       </c>
@@ -1591,19 +1591,19 @@
       <c r="I32" s="12">
         <v>42762.708333333336</v>
       </c>
-      <c r="J32" s="50"/>
+      <c r="J32" s="41"/>
     </row>
     <row r="33" spans="1:10">
-      <c r="A33" s="45">
+      <c r="A33" s="37">
         <v>32</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
-      <c r="E33" s="22" t="s">
+      <c r="E33" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="F33" s="22"/>
+      <c r="F33" s="59"/>
       <c r="G33" s="15" t="s">
         <v>30</v>
       </c>
@@ -1613,10 +1613,10 @@
       <c r="I33" s="4">
         <v>42762.708333333336</v>
       </c>
-      <c r="J33" s="51"/>
+      <c r="J33" s="42"/>
     </row>
     <row r="34" spans="1:10">
-      <c r="A34" s="45">
+      <c r="A34" s="37">
         <v>33</v>
       </c>
       <c r="B34" s="10"/>
@@ -1635,10 +1635,10 @@
       <c r="I34" s="12">
         <v>42755.708333333336</v>
       </c>
-      <c r="J34" s="50"/>
+      <c r="J34" s="41"/>
     </row>
     <row r="35" spans="1:10">
-      <c r="A35" s="45">
+      <c r="A35" s="37">
         <v>34</v>
       </c>
       <c r="B35" s="2"/>
@@ -1657,23 +1657,23 @@
       <c r="I35" s="4">
         <v>42762.708333333336</v>
       </c>
-      <c r="J35" s="51">
+      <c r="J35" s="42">
         <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:10">
-      <c r="A36" s="45">
+      <c r="A36" s="37">
         <v>35</v>
       </c>
       <c r="B36" s="10"/>
       <c r="C36" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="D36" s="23" t="s">
+      <c r="D36" s="58" t="s">
         <v>62</v>
       </c>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
+      <c r="E36" s="58"/>
+      <c r="F36" s="58"/>
       <c r="G36" s="14" t="s">
         <v>7</v>
       </c>
@@ -1683,10 +1683,10 @@
       <c r="I36" s="12">
         <v>42762.708333333336</v>
       </c>
-      <c r="J36" s="50"/>
+      <c r="J36" s="41"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="45">
+      <c r="A37" s="37">
         <v>36</v>
       </c>
       <c r="B37" s="2"/>
@@ -1705,10 +1705,10 @@
       <c r="I37" s="4">
         <v>42755.708333333336</v>
       </c>
-      <c r="J37" s="51"/>
+      <c r="J37" s="42"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="45">
+      <c r="A38" s="37">
         <v>37</v>
       </c>
       <c r="B38" s="10"/>
@@ -1727,19 +1727,19 @@
       <c r="I38" s="12">
         <v>42762.708333333336</v>
       </c>
-      <c r="J38" s="50"/>
+      <c r="J38" s="41"/>
     </row>
     <row r="39" spans="1:10">
-      <c r="A39" s="45">
+      <c r="A39" s="37">
         <v>38</v>
       </c>
       <c r="B39" s="5"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="21" t="s">
+      <c r="D39" s="63" t="s">
         <v>51</v>
       </c>
-      <c r="E39" s="21"/>
-      <c r="F39" s="21"/>
+      <c r="E39" s="63"/>
+      <c r="F39" s="63"/>
       <c r="G39" s="16" t="s">
         <v>49</v>
       </c>
@@ -1749,10 +1749,16 @@
       <c r="I39" s="7">
         <v>42765.708333333336</v>
       </c>
-      <c r="J39" s="55"/>
+      <c r="J39" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D27:F27"/>
     <mergeCell ref="L1:M1"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="D30:F30"/>
@@ -1767,12 +1773,6 @@
     <mergeCell ref="C3:F3"/>
     <mergeCell ref="D4:F4"/>
     <mergeCell ref="D6:F6"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="D27:F27"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>